<commit_message>
feat: Replace dynamic charts with server-rendered static charts
- Add Plotly-based chart generation in Python API (chart_generator.py)
- Generate 7 MSA charts as base64 PNG images server-side
- Add StaticChartDisplay component for rendering static charts
- Update ChatMessage to detect and render static vs dynamic charts
- Add plotly>=5.18.0 and kaleido>=0.2.1 dependencies
- Fix chart label positioning for R and X-bar control charts
- Add high-contrast colors for interaction plot
- Include various UI and auth component updates

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/templates/plantilla-msa.xlsx
+++ b/public/templates/plantilla-msa.xlsx
@@ -1,52 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
   <sheets>
-    <sheet name="MSA Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,13 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -150,7 +199,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -185,7 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -220,16 +267,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -351,594 +402,623 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Part</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Operator</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Measurement 1</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Measurement 2</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Measurement 3</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Pieza</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Operador</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Medición 1</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Medición 2</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Medición 3</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <v>A</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>9.891</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>9.964</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>9.962</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="str">
-        <v>B</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>9.923</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>9.895</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>9.863</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="str">
-        <v>C</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>9.847</v>
       </c>
-      <c r="D4">
-        <v>9.954</v>
-      </c>
-      <c r="E4">
+      <c r="D4" t="n">
+        <v>9.954000000000001</v>
+      </c>
+      <c r="E4" t="n">
         <v>9.898</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" t="n">
         <v>2</v>
       </c>
-      <c r="B5" t="str">
-        <v>A</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>9.93</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>9.885</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>9.898</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" t="n">
         <v>2</v>
       </c>
-      <c r="B6" t="str">
-        <v>B</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>9.913</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="n">
         <v>9.972</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>9.933</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7" t="n">
         <v>2</v>
       </c>
-      <c r="B7" t="str">
-        <v>C</v>
-      </c>
-      <c r="C7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>9.914</v>
       </c>
-      <c r="D7">
-        <v>9.867</v>
-      </c>
-      <c r="E7">
-        <v>9.979</v>
+      <c r="D7" t="n">
+        <v>9.867000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>9.978999999999999</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" t="n">
         <v>3</v>
       </c>
-      <c r="B8" t="str">
-        <v>A</v>
-      </c>
-      <c r="C8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>10.006</v>
       </c>
-      <c r="D8">
-        <v>9.893</v>
-      </c>
-      <c r="E8">
+      <c r="D8" t="n">
+        <v>9.893000000000001</v>
+      </c>
+      <c r="E8" t="n">
         <v>9.895</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" t="n">
         <v>3</v>
       </c>
-      <c r="B9" t="str">
-        <v>B</v>
-      </c>
-      <c r="C9">
-        <v>9.986</v>
-      </c>
-      <c r="D9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>9.986000000000001</v>
+      </c>
+      <c r="D9" t="n">
         <v>9.952</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>9.949</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" t="n">
         <v>3</v>
       </c>
-      <c r="B10" t="str">
-        <v>C</v>
-      </c>
-      <c r="C10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>9.958</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>9.939</v>
       </c>
-      <c r="E10">
-        <v>9.953</v>
+      <c r="E10" t="n">
+        <v>9.952999999999999</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" t="n">
         <v>4</v>
       </c>
-      <c r="B11" t="str">
-        <v>A</v>
-      </c>
-      <c r="C11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
         <v>10.017</v>
       </c>
-      <c r="D11">
-        <v>9.982</v>
-      </c>
-      <c r="E11">
-        <v>9.951</v>
+      <c r="D11" t="n">
+        <v>9.981999999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9.951000000000001</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" t="n">
         <v>4</v>
       </c>
-      <c r="B12" t="str">
-        <v>B</v>
-      </c>
-      <c r="C12">
-        <v>9.944</v>
-      </c>
-      <c r="D12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>9.944000000000001</v>
+      </c>
+      <c r="D12" t="n">
         <v>9.917</v>
       </c>
-      <c r="E12">
-        <v>9.905</v>
+      <c r="E12" t="n">
+        <v>9.904999999999999</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" t="n">
         <v>4</v>
       </c>
-      <c r="B13" t="str">
-        <v>C</v>
-      </c>
-      <c r="C13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>9.943</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="n">
         <v>9.971</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>10.009</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
+      <c r="A14" t="n">
         <v>5</v>
       </c>
-      <c r="B14" t="str">
-        <v>A</v>
-      </c>
-      <c r="C14">
-        <v>9.953</v>
-      </c>
-      <c r="D14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>9.952999999999999</v>
+      </c>
+      <c r="D14" t="n">
         <v>10.047</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>9.993</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="str">
+      <c r="A15" t="n">
         <v>5</v>
       </c>
-      <c r="B15" t="str">
-        <v>B</v>
-      </c>
-      <c r="C15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>10.03</v>
       </c>
-      <c r="D15">
-        <v>9.931</v>
-      </c>
-      <c r="E15">
+      <c r="D15" t="n">
+        <v>9.930999999999999</v>
+      </c>
+      <c r="E15" t="n">
         <v>9.932</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="str">
+      <c r="A16" t="n">
         <v>5</v>
       </c>
-      <c r="B16" t="str">
-        <v>C</v>
-      </c>
-      <c r="C16">
-        <v>9.967</v>
-      </c>
-      <c r="D16">
-        <v>9.95</v>
-      </c>
-      <c r="E16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>9.967000000000001</v>
+      </c>
+      <c r="D16" t="n">
+        <v>9.949999999999999</v>
+      </c>
+      <c r="E16" t="n">
         <v>10.021</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="str">
+      <c r="A17" t="n">
         <v>6</v>
       </c>
-      <c r="B17" t="str">
-        <v>A</v>
-      </c>
-      <c r="C17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
         <v>9.972</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="n">
         <v>9.956</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>9.959</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
+      <c r="A18" t="n">
         <v>6</v>
       </c>
-      <c r="B18" t="str">
-        <v>B</v>
-      </c>
-      <c r="C18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
         <v>10.003</v>
       </c>
-      <c r="D18">
-        <v>9.982</v>
-      </c>
-      <c r="E18">
+      <c r="D18" t="n">
+        <v>9.981999999999999</v>
+      </c>
+      <c r="E18" t="n">
         <v>10.02</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
+      <c r="A19" t="n">
         <v>6</v>
       </c>
-      <c r="B19" t="str">
-        <v>C</v>
-      </c>
-      <c r="C19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>9.993</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="n">
         <v>10.014</v>
       </c>
-      <c r="E19">
-        <v>9.954</v>
+      <c r="E19" t="n">
+        <v>9.954000000000001</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="str">
+      <c r="A20" t="n">
         <v>7</v>
       </c>
-      <c r="B20" t="str">
-        <v>A</v>
-      </c>
-      <c r="C20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
         <v>10.053</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="n">
         <v>10.069</v>
       </c>
-      <c r="E20">
-        <v>9.979</v>
+      <c r="E20" t="n">
+        <v>9.978999999999999</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="str">
+      <c r="A21" t="n">
         <v>7</v>
       </c>
-      <c r="B21" t="str">
-        <v>B</v>
-      </c>
-      <c r="C21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
         <v>9.984</v>
       </c>
-      <c r="D21">
-        <v>9.989</v>
-      </c>
-      <c r="E21">
+      <c r="D21" t="n">
+        <v>9.989000000000001</v>
+      </c>
+      <c r="E21" t="n">
         <v>10.05</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="str">
+      <c r="A22" t="n">
         <v>7</v>
       </c>
-      <c r="B22" t="str">
-        <v>C</v>
-      </c>
-      <c r="C22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
         <v>9.993</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>10.054</v>
       </c>
-      <c r="E22">
+      <c r="E22" t="n">
         <v>10.083</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="str">
+      <c r="A23" t="n">
         <v>8</v>
       </c>
-      <c r="B23" t="str">
-        <v>A</v>
-      </c>
-      <c r="C23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
         <v>10.047</v>
       </c>
-      <c r="D23">
-        <v>9.992</v>
-      </c>
-      <c r="E23">
+      <c r="D23" t="n">
+        <v>9.992000000000001</v>
+      </c>
+      <c r="E23" t="n">
         <v>10.021</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="str">
+      <c r="A24" t="n">
         <v>8</v>
       </c>
-      <c r="B24" t="str">
-        <v>B</v>
-      </c>
-      <c r="C24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
         <v>10.026</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="n">
         <v>10.034</v>
       </c>
-      <c r="E24">
+      <c r="E24" t="n">
         <v>10.001</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="str">
+      <c r="A25" t="n">
         <v>8</v>
       </c>
-      <c r="B25" t="str">
-        <v>C</v>
-      </c>
-      <c r="C25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
         <v>10.012</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="n">
         <v>10.031</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="n">
         <v>10.103</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="str">
+      <c r="A26" t="n">
         <v>9</v>
       </c>
-      <c r="B26" t="str">
-        <v>A</v>
-      </c>
-      <c r="C26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
         <v>10.103</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>10.081</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>10.045</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="str">
+      <c r="A27" t="n">
         <v>9</v>
       </c>
-      <c r="B27" t="str">
-        <v>B</v>
-      </c>
-      <c r="C27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
         <v>10.04</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>10.08</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>10.026</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="str">
+      <c r="A28" t="n">
         <v>9</v>
       </c>
-      <c r="B28" t="str">
-        <v>C</v>
-      </c>
-      <c r="C28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
         <v>10.099</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>10.079</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="n">
         <v>10.078</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="str">
+      <c r="A29" t="n">
         <v>10</v>
       </c>
-      <c r="B29" t="str">
-        <v>A</v>
-      </c>
-      <c r="C29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
         <v>10.075</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="n">
         <v>10.094</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>10.052</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="str">
+      <c r="A30" t="n">
         <v>10</v>
       </c>
-      <c r="B30" t="str">
-        <v>B</v>
-      </c>
-      <c r="C30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
         <v>10.124</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="n">
         <v>10.052</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="n">
         <v>10.056</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="str">
+      <c r="A31" t="n">
         <v>10</v>
       </c>
-      <c r="B31" t="str">
-        <v>C</v>
-      </c>
-      <c r="C31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
         <v>10.086</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>10.032</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>10.031</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E31"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>